<commit_message>
remove heading of key column (to make it even more realistically)
</commit_message>
<xml_diff>
--- a/WorkbookImporter.Specs/SampleFiles/RealisticTemplateFilled.xlsx
+++ b/WorkbookImporter.Specs/SampleFiles/RealisticTemplateFilled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulroho/Repos/evaluation/Evaluate.MiniExcel/WorkbookImporter.Specs/SampleFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CA1BE52-A40C-E145-8BA7-BED9FAE968B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF536EB-11CA-8E40-AA1B-71F4539A0C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="mm7/Eq4iI1Om+VpWkofcL0Yb2+fb7IaYMworlGdtfVze6H8MmcAwXNInDCaewPpRKyU5fp3o75pdZ04RD3qimg==" workbookSaltValue="5ooB9URIntRNZl2FUNYmOw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{5DBEFA01-1099-B549-8184-7627E4DA045F}"/>
@@ -18,7 +18,7 @@
     <sheet name="Important Sheet" sheetId="1" r:id="rId2"/>
     <sheet name="Additional Sheet" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Header Text 1</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Section A</t>
-  </si>
-  <si>
-    <t>The Key</t>
   </si>
   <si>
     <t>The Value</t>
@@ -1226,7 +1223,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
@@ -1234,7 +1231,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1250,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A86B12B-C8EB-7F47-BDED-A8237C4CF19D}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="171" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="171" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1268,13 +1265,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" s="59" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -1284,35 +1281,33 @@
     </row>
     <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="46"/>
       <c r="D5" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49" t="s">
         <v>5</v>
-      </c>
-      <c r="F5" s="49" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="64" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="50"/>
       <c r="D6" s="53" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1322,31 +1317,31 @@
         <v>1</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="52"/>
       <c r="D8" s="57" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="43">
         <v>987</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1356,13 +1351,13 @@
         <v>3</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="9">
         <v>46014</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1378,75 +1373,73 @@
     </row>
     <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="F12" s="25" t="s">
         <v>5</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="80"/>
       <c r="C14" s="17"/>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="11">
         <v>2.2200000000000002</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" s="21">
         <v>3.3330000000000002</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:7" s="59" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="77"/>
       <c r="D17" s="77"/>
@@ -1456,109 +1449,107 @@
     </row>
     <row r="18" spans="2:7" ht="17" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="35"/>
+      <c r="F18" s="29" t="s">
         <v>5</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="17" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B19" s="70" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F19" s="13">
         <v>555.54999999999995</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="17" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="71"/>
       <c r="C20" s="68"/>
       <c r="D20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20" s="11">
         <v>44.44</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="17" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B21" s="71"/>
       <c r="C21" s="69" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" s="15">
         <v>3.33</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="17" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="72"/>
       <c r="C22" s="68"/>
       <c r="D22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22" s="11">
         <v>2.2000000000000002</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="40"/>
       <c r="D23" s="41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="21">
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zspNkIo912oU/LaEqlP9P18KmLe8MpgkpmnvD2QGPF1G8BW81d5oROWpr2P/G5SZkZCddaTr5ygsqbmJYP2Dvw==" saltValue="d1F9yEBOjX5g7jB9x6GMUA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="sIkL8ILwhzIr3xxjbchH1yWDGkFKBxyoit92UbFduCPHu3cyjx1C7Y/6qxpQOnDUJNbRYgQ11jkBTM2mFEwJJg==" saltValue="caHvJTvBJm6WTcv35Av5iA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="9">
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B6:B7"/>
@@ -1614,22 +1605,22 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="5"/>
     </row>

</xml_diff>